<commit_message>
updated cuz it be 2019
</commit_message>
<xml_diff>
--- a/Documents/I-O List.xlsx
+++ b/Documents/I-O List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="9555" windowHeight="9720"/>
@@ -11,12 +11,12 @@
     <sheet name="Raspberry Pi" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -144,24 +144,6 @@
     <t>Relay_10</t>
   </si>
   <si>
-    <t>Relay_11</t>
-  </si>
-  <si>
-    <t>Relay_12</t>
-  </si>
-  <si>
-    <t>Relay_13</t>
-  </si>
-  <si>
-    <t>Relay_14</t>
-  </si>
-  <si>
-    <t>Relay_15</t>
-  </si>
-  <si>
-    <t>Relay_16</t>
-  </si>
-  <si>
     <t>Pump Power</t>
   </si>
   <si>
@@ -199,6 +181,18 @@
   </si>
   <si>
     <t>Digital closure</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Yellow LED</t>
+  </si>
+  <si>
+    <t>Purple LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
   </si>
 </sst>
 </file>
@@ -537,10 +531,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,10 +560,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
@@ -576,141 +573,36 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -726,10 +618,10 @@
         <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -746,10 +638,10 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -766,131 +658,41 @@
         <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -906,10 +708,10 @@
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -926,10 +728,10 @@
         <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -946,10 +748,10 @@
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -966,10 +768,10 @@
         <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -986,10 +788,10 @@
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1006,10 +808,10 @@
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1026,10 +828,10 @@
         <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1046,7 +848,7 @@
         <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
         <v>18</v>
@@ -1066,7 +868,7 @@
         <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F26" t="s">
         <v>18</v>
@@ -1086,7 +888,7 @@
         <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F27" t="s">
         <v>18</v>
@@ -1106,7 +908,7 @@
         <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F28" t="s">
         <v>18</v>
@@ -1117,77 +919,194 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>49</v>
-      </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1201,78 +1120,19 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>